<commit_message>
finalized analysis script and begin to structure the manuscript using RMarkdown
</commit_message>
<xml_diff>
--- a/experiment_setup/condition_participant/ConditionFIle_Mirror_Block1_1.xlsx
+++ b/experiment_setup/condition_participant/ConditionFIle_Mirror_Block1_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dani/Desktop/MirrorExp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8987251e2c38395f/Dokumente/Studium/4_Semester/PsyBSc14_Grundlagen_der_Psychologie_Vertiefung/scene_orientation_repetition_priming/experiment_setup/condition_participant/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB956B0E-2C4B-B840-BF5F-64D1A827F157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{CB956B0E-2C4B-B840-BF5F-64D1A827F157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BD13FDF-2D88-D748-B13F-9B79FEBDB61C}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{03C06B8E-1EE1-DF47-854E-AF5A2E25C450}"/>
+    <workbookView xWindow="-38400" yWindow="-1880" windowWidth="38400" windowHeight="21600" xr2:uid="{03C06B8E-1EE1-DF47-854E-AF5A2E25C450}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -192,7 +192,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -208,7 +208,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -507,7 +507,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>